<commit_message>
create files as described in notebook
</commit_message>
<xml_diff>
--- a/notebooks/wip/Multi-strain model/Strain Information.xlsx
+++ b/notebooks/wip/Multi-strain model/Strain Information.xlsx
@@ -35,24 +35,9 @@
     <t>Physiology</t>
   </si>
   <si>
-    <t xml:space="preserve">CP016552.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP020030.1 </t>
-  </si>
-  <si>
     <t>CP012712.1</t>
   </si>
   <si>
-    <t xml:space="preserve">CP002835.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP001638 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP008903.1 </t>
-  </si>
-  <si>
     <t>Geobacillus sp. LC300</t>
   </si>
   <si>
@@ -75,6 +60,21 @@
   </si>
   <si>
     <t>Geobacillus stearothermophilus DSM 458</t>
+  </si>
+  <si>
+    <t>CP016552.1</t>
+  </si>
+  <si>
+    <t>CP020030.1</t>
+  </si>
+  <si>
+    <t>CP002835.1</t>
+  </si>
+  <si>
+    <t>CP001638</t>
+  </si>
+  <si>
+    <t>CP008903.1</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -436,73 +436,73 @@
     </row>
     <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Compare NCIMB11955 to M10exg
</commit_message>
<xml_diff>
--- a/notebooks/wip/Multi-strain model/Strain Information.xlsx
+++ b/notebooks/wip/Multi-strain model/Strain Information.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Strain</t>
   </si>
@@ -35,46 +35,10 @@
     <t>Physiology</t>
   </si>
   <si>
-    <t>CP012712.1</t>
-  </si>
-  <si>
-    <t>Geobacillus sp. LC300</t>
-  </si>
-  <si>
-    <t>Obligate aerobe</t>
-  </si>
-  <si>
-    <t>Geobacillus sp. WCH70</t>
-  </si>
-  <si>
-    <t>Parageobacillus thermoglucosidasius C56-YS93</t>
-  </si>
-  <si>
     <t>Facultative anaerobe</t>
   </si>
   <si>
-    <t>Parageobacillus thermoglucosidasius DSM 2542</t>
-  </si>
-  <si>
-    <t>Geobacillus thermodenitrificans T12</t>
-  </si>
-  <si>
-    <t>Geobacillus stearothermophilus DSM 458</t>
-  </si>
-  <si>
-    <t>CP016552.1</t>
-  </si>
-  <si>
-    <t>CP020030.1</t>
-  </si>
-  <si>
-    <t>CP002835.1</t>
-  </si>
-  <si>
-    <t>CP001638</t>
-  </si>
-  <si>
-    <t>CP008903.1</t>
+    <t>Goebacillus thermoglucosidasius M10EXG</t>
   </si>
 </sst>
 </file>
@@ -409,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -436,81 +400,15 @@
     </row>
     <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2501416905</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>